<commit_message>
Updated rune crafter and inspector to show first order construction of sigils
</commit_message>
<xml_diff>
--- a/runeCrafterAgenda.xlsx
+++ b/runeCrafterAgenda.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t xml:space="preserve">Step</t>
   </si>
@@ -33,16 +33,28 @@
     <t xml:space="preserve">Due Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Trash inspected thing to clear inspector</t>
+    <t xml:space="preserve">Update Rune Crafter Frame</t>
   </si>
   <si>
     <t xml:space="preserve">Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">Place 1 level deeper representation of sigils in both inspector and Rune Crafter (show both γ and (α u β) )</t>
+    <t xml:space="preserve">Trash inspected thing to clear inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleanup Styles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rewrite back-end naming of sets</t>
   </si>
   <si>
     <t xml:space="preserve">Ryan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create different tools for each kind of rune crafting, with different frames</t>
   </si>
   <si>
     <t xml:space="preserve">Task</t>
@@ -58,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Render completed rune tree upon creating rune that matches the runic key/display victory msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place 1 level deeper representation of sigils in both inspector and Rune Crafter (show both γ and (α u β) )</t>
   </si>
   <si>
     <t xml:space="preserve">Ashish</t>
@@ -223,7 +238,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,23 +286,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF7F0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left style="thin"/>
-        <right style="thin"/>
-        <top/>
-        <bottom style="thin"/>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF600000"/>
         </patternFill>
       </fill>
@@ -312,6 +310,23 @@
         <left style="thin"/>
         <right style="thin"/>
         <top style="thin"/>
+        <bottom style="thin"/>
+        <diagonal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7F0000"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="false" diagonalDown="false">
+        <left style="thin"/>
+        <right style="thin"/>
+        <top/>
         <bottom style="thin"/>
         <diagonal/>
       </border>
@@ -388,15 +403,15 @@
   <dimension ref="A1:C499"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,42 +425,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="n">
-        <v>42581</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="7" t="n">
+        <v>42582</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="n">
-        <v>42588</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
@@ -2913,21 +2946,6 @@
       <c r="C499" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>AND(Assignments!C3 - TODAY() &lt; 0, Assignments!A3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(Assignments!C3 - TODAY() &lt; 0, Assignments!A3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND(Assignments!C3 - TODAY() &lt; 0, Assignments!A3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2946,38 +2964,38 @@
   <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="14" t="n">
         <v>42578</v>
@@ -2989,10 +3007,10 @@
     </row>
     <row r="3" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="9" t="n">
         <v>42581</v>
@@ -3002,10 +3020,19 @@
         <v>42579</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="16" t="str">
+    <row r="4" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>42588</v>
+      </c>
+      <c r="D4" s="16" t="n">
         <f aca="true">IF(Completed!A4&lt;&gt;"", IF(Completed!D4="", TODAY(), Completed!D4), "")</f>
-        <v/>
+        <v>42581</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4485,17 +4512,17 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
+  <conditionalFormatting sqref="B2">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(Completed!C2 - TODAY() &lt; 0, Completed!A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
+  <conditionalFormatting sqref="C2">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(Completed!C2 - TODAY() &lt; 0, Completed!A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
+  <conditionalFormatting sqref="A2">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(Completed!C2 - TODAY() &lt; 0, Completed!A2&lt;&gt;"")</formula>
     </cfRule>
@@ -4523,12 +4550,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4538,7 +4565,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the forge to automatically craft the relevant runes
</commit_message>
<xml_diff>
--- a/runeCrafterAgenda.xlsx
+++ b/runeCrafterAgenda.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t xml:space="preserve">Step</t>
   </si>
@@ -33,19 +33,16 @@
     <t xml:space="preserve">Due Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Update Rune Crafter Frame</t>
+    <t xml:space="preserve">Trash inspected thing to clear inspector</t>
   </si>
   <si>
     <t xml:space="preserve">Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">Trash inspected thing to clear inspector</t>
+    <t xml:space="preserve">Cleanup Styles</t>
   </si>
   <si>
     <t xml:space="preserve">????</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleanup Styles</t>
   </si>
   <si>
     <t xml:space="preserve">Rewrite back-end naming of sets</t>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Place 1 level deeper representation of sigils in both inspector and Rune Crafter (show both γ and (α u β) )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Rune Crafter Frame</t>
   </si>
   <si>
     <t xml:space="preserve">Ashish</t>
@@ -226,19 +226,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,18 +400,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C499"/>
+  <dimension ref="A1:C498"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,7 +425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -433,10 +433,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>42582</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -447,38 +447,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
@@ -2939,11 +2933,6 @@
       <c r="A498" s="6"/>
       <c r="B498" s="6"/>
       <c r="C498" s="7"/>
-    </row>
-    <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="8"/>
-      <c r="B499" s="8"/>
-      <c r="C499" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2964,38 +2953,38 @@
   <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="14" t="n">
         <v>42578</v>
@@ -3006,13 +2995,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="9" t="n">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="n">
         <v>42581</v>
       </c>
       <c r="D3" s="16" t="n">
@@ -3021,13 +3010,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7" t="n">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="n">
         <v>42588</v>
       </c>
       <c r="D4" s="16" t="n">
@@ -3035,10 +3024,19 @@
         <v>42581</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="16" t="str">
+    <row r="5" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>42582</v>
+      </c>
+      <c r="D5" s="16" t="n">
         <f aca="true">IF(Completed!A5&lt;&gt;"", IF(Completed!D5="", TODAY(), Completed!D5), "")</f>
-        <v/>
+        <v>42585</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4550,12 +4548,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added space for recipes in rune crafter, with first recipe image
</commit_message>
<xml_diff>
--- a/runeCrafterAgenda.xlsx
+++ b/runeCrafterAgenda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\tutorial2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\mathGame\tutorial2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Completed" sheetId="2" r:id="rId2"/>
     <sheet name="DropDowns" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" iterate="1" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Step</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Ryan</t>
-  </si>
-  <si>
-    <t>Create different tools for each kind of rune crafting, with different frames</t>
   </si>
   <si>
     <t>Task</t>
@@ -80,6 +77,21 @@
   </si>
   <si>
     <t>Trashable inspector</t>
+  </si>
+  <si>
+    <t>Create images for remaining 7 Recipes</t>
+  </si>
+  <si>
+    <t>14/08/16</t>
+  </si>
+  <si>
+    <t>Set drag data for recipes</t>
+  </si>
+  <si>
+    <t>Craft 1st rune type with 1st recipe</t>
+  </si>
+  <si>
+    <t>Team</t>
   </si>
 </sst>
 </file>
@@ -694,18 +706,18 @@
   <dimension ref="A1:AMK497"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" style="1"/>
-    <col min="2" max="2" width="16.81640625" style="1"/>
-    <col min="3" max="3" width="15.7265625" style="1"/>
-    <col min="4" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="31.85546875" style="1"/>
+    <col min="2" max="2" width="16.85546875" style="1"/>
+    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="4" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -716,7 +728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -727,7 +739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -738,2478 +750,2490 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="9"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="9"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="9"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="7"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="7"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="9"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="7"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="9"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="7"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="9"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="7"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="9"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="7"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="9"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="7"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="9"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="9"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="9"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="7"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="9"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="7"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="7"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="9"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="9"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="7"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="9"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="9"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="7"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="9"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="7"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="7"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="9"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="7"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
       <c r="C90" s="9"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="7"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="9"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="7"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="9"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="7"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="9"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="7"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="9"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="7"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="9"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="7"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="9"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="7"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="9"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="7"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="8"/>
       <c r="B106" s="8"/>
       <c r="C106" s="9"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="7"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="9"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="7"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="9"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="7"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="C112" s="9"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="7"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="8"/>
       <c r="B114" s="8"/>
       <c r="C114" s="9"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="7"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="7"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="9"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="7"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="8"/>
       <c r="B120" s="8"/>
       <c r="C120" s="9"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="7"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="9"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="7"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="9"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="7"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="8"/>
       <c r="B126" s="8"/>
       <c r="C126" s="9"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="C127" s="7"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="8"/>
       <c r="B128" s="8"/>
       <c r="C128" s="9"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="7"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="8"/>
       <c r="B130" s="8"/>
       <c r="C130" s="9"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="6"/>
       <c r="B131" s="6"/>
       <c r="C131" s="7"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="8"/>
       <c r="B132" s="8"/>
       <c r="C132" s="9"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="C133" s="7"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="8"/>
       <c r="B134" s="8"/>
       <c r="C134" s="9"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="6"/>
       <c r="B135" s="6"/>
       <c r="C135" s="7"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="9"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
       <c r="B137" s="6"/>
       <c r="C137" s="7"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="9"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="6"/>
       <c r="B139" s="6"/>
       <c r="C139" s="7"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="8"/>
       <c r="B140" s="8"/>
       <c r="C140" s="9"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="C141" s="7"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="9"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
       <c r="B143" s="6"/>
       <c r="C143" s="7"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="9"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
       <c r="B145" s="6"/>
       <c r="C145" s="7"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="9"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
       <c r="B147" s="6"/>
       <c r="C147" s="7"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="9"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
       <c r="B149" s="6"/>
       <c r="C149" s="7"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="8"/>
       <c r="B150" s="8"/>
       <c r="C150" s="9"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
       <c r="C151" s="7"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="8"/>
       <c r="B152" s="8"/>
       <c r="C152" s="9"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="6"/>
       <c r="B153" s="6"/>
       <c r="C153" s="7"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="9"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="C155" s="7"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="9"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="C157" s="7"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="8"/>
       <c r="B158" s="8"/>
       <c r="C158" s="9"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="7"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="8"/>
       <c r="B160" s="8"/>
       <c r="C160" s="9"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="6"/>
       <c r="B161" s="6"/>
       <c r="C161" s="7"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="9"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="7"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="8"/>
       <c r="B164" s="8"/>
       <c r="C164" s="9"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="6"/>
       <c r="B165" s="6"/>
       <c r="C165" s="7"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="8"/>
       <c r="B166" s="8"/>
       <c r="C166" s="9"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="6"/>
       <c r="B167" s="6"/>
       <c r="C167" s="7"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="8"/>
       <c r="B168" s="8"/>
       <c r="C168" s="9"/>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="C169" s="7"/>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="8"/>
       <c r="B170" s="8"/>
       <c r="C170" s="9"/>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="7"/>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="8"/>
       <c r="B172" s="8"/>
       <c r="C172" s="9"/>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="C173" s="7"/>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="8"/>
       <c r="B174" s="8"/>
       <c r="C174" s="9"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="7"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="8"/>
       <c r="B176" s="8"/>
       <c r="C176" s="9"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="6"/>
       <c r="B177" s="6"/>
       <c r="C177" s="7"/>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="C178" s="9"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="6"/>
       <c r="B179" s="6"/>
       <c r="C179" s="7"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="8"/>
       <c r="B180" s="8"/>
       <c r="C180" s="9"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="6"/>
       <c r="B181" s="6"/>
       <c r="C181" s="7"/>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="C182" s="9"/>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="6"/>
       <c r="B183" s="6"/>
       <c r="C183" s="7"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="C184" s="9"/>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="7"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="C186" s="9"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="6"/>
       <c r="B187" s="6"/>
       <c r="C187" s="7"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="C188" s="9"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="6"/>
       <c r="B189" s="6"/>
       <c r="C189" s="7"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="8"/>
       <c r="B190" s="8"/>
       <c r="C190" s="9"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="6"/>
       <c r="B191" s="6"/>
       <c r="C191" s="7"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="8"/>
       <c r="B192" s="8"/>
       <c r="C192" s="9"/>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="6"/>
       <c r="B193" s="6"/>
       <c r="C193" s="7"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="C194" s="9"/>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="6"/>
       <c r="B195" s="6"/>
       <c r="C195" s="7"/>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
       <c r="C196" s="9"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="6"/>
       <c r="B197" s="6"/>
       <c r="C197" s="7"/>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="8"/>
       <c r="B198" s="8"/>
       <c r="C198" s="9"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="6"/>
       <c r="B199" s="6"/>
       <c r="C199" s="7"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="8"/>
       <c r="B200" s="8"/>
       <c r="C200" s="9"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="6"/>
       <c r="B201" s="6"/>
       <c r="C201" s="7"/>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="C202" s="9"/>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="6"/>
       <c r="B203" s="6"/>
       <c r="C203" s="7"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="8"/>
       <c r="B204" s="8"/>
       <c r="C204" s="9"/>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="C205" s="7"/>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="8"/>
       <c r="B206" s="8"/>
       <c r="C206" s="9"/>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="6"/>
       <c r="B207" s="6"/>
       <c r="C207" s="7"/>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="8"/>
       <c r="B208" s="8"/>
       <c r="C208" s="9"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
       <c r="C209" s="7"/>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="8"/>
       <c r="B210" s="8"/>
       <c r="C210" s="9"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="C211" s="7"/>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="8"/>
       <c r="B212" s="8"/>
       <c r="C212" s="9"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="C213" s="7"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="8"/>
       <c r="B214" s="8"/>
       <c r="C214" s="9"/>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
       <c r="C215" s="7"/>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="8"/>
       <c r="B216" s="8"/>
       <c r="C216" s="9"/>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="C217" s="7"/>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="8"/>
       <c r="B218" s="8"/>
       <c r="C218" s="9"/>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="C219" s="7"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="8"/>
       <c r="B220" s="8"/>
       <c r="C220" s="9"/>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="C221" s="7"/>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="8"/>
       <c r="B222" s="8"/>
       <c r="C222" s="9"/>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="C223" s="7"/>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="8"/>
       <c r="B224" s="8"/>
       <c r="C224" s="9"/>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="6"/>
       <c r="B225" s="6"/>
       <c r="C225" s="7"/>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="8"/>
       <c r="B226" s="8"/>
       <c r="C226" s="9"/>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="6"/>
       <c r="B227" s="6"/>
       <c r="C227" s="7"/>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="8"/>
       <c r="B228" s="8"/>
       <c r="C228" s="9"/>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="6"/>
       <c r="B229" s="6"/>
       <c r="C229" s="7"/>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="8"/>
       <c r="B230" s="8"/>
       <c r="C230" s="9"/>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="7"/>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="8"/>
       <c r="B232" s="8"/>
       <c r="C232" s="9"/>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="6"/>
       <c r="B233" s="6"/>
       <c r="C233" s="7"/>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="8"/>
       <c r="B234" s="8"/>
       <c r="C234" s="9"/>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="6"/>
       <c r="B235" s="6"/>
       <c r="C235" s="7"/>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="8"/>
       <c r="B236" s="8"/>
       <c r="C236" s="9"/>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="6"/>
       <c r="B237" s="6"/>
       <c r="C237" s="7"/>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="8"/>
       <c r="B238" s="8"/>
       <c r="C238" s="9"/>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="6"/>
       <c r="B239" s="6"/>
       <c r="C239" s="7"/>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="8"/>
       <c r="B240" s="8"/>
       <c r="C240" s="9"/>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="6"/>
       <c r="B241" s="6"/>
       <c r="C241" s="7"/>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="8"/>
       <c r="B242" s="8"/>
       <c r="C242" s="9"/>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="6"/>
       <c r="B243" s="6"/>
       <c r="C243" s="7"/>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="8"/>
       <c r="B244" s="8"/>
       <c r="C244" s="9"/>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="6"/>
       <c r="B245" s="6"/>
       <c r="C245" s="7"/>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="8"/>
       <c r="B246" s="8"/>
       <c r="C246" s="9"/>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="6"/>
       <c r="B247" s="6"/>
       <c r="C247" s="7"/>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="8"/>
       <c r="B248" s="8"/>
       <c r="C248" s="9"/>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="C249" s="7"/>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="8"/>
       <c r="B250" s="8"/>
       <c r="C250" s="9"/>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="6"/>
       <c r="B251" s="6"/>
       <c r="C251" s="7"/>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="8"/>
       <c r="B252" s="8"/>
       <c r="C252" s="9"/>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="6"/>
       <c r="B253" s="6"/>
       <c r="C253" s="7"/>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="8"/>
       <c r="B254" s="8"/>
       <c r="C254" s="9"/>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="6"/>
       <c r="B255" s="6"/>
       <c r="C255" s="7"/>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="8"/>
       <c r="B256" s="8"/>
       <c r="C256" s="9"/>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="6"/>
       <c r="B257" s="6"/>
       <c r="C257" s="7"/>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="8"/>
       <c r="B258" s="8"/>
       <c r="C258" s="9"/>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="6"/>
       <c r="B259" s="6"/>
       <c r="C259" s="7"/>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="8"/>
       <c r="B260" s="8"/>
       <c r="C260" s="9"/>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="6"/>
       <c r="B261" s="6"/>
       <c r="C261" s="7"/>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="8"/>
       <c r="B262" s="8"/>
       <c r="C262" s="9"/>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="6"/>
       <c r="B263" s="6"/>
       <c r="C263" s="7"/>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="8"/>
       <c r="B264" s="8"/>
       <c r="C264" s="9"/>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="C265" s="7"/>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="8"/>
       <c r="B266" s="8"/>
       <c r="C266" s="9"/>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="6"/>
       <c r="B267" s="6"/>
       <c r="C267" s="7"/>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="8"/>
       <c r="B268" s="8"/>
       <c r="C268" s="9"/>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="6"/>
       <c r="B269" s="6"/>
       <c r="C269" s="7"/>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="8"/>
       <c r="B270" s="8"/>
       <c r="C270" s="9"/>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="6"/>
       <c r="B271" s="6"/>
       <c r="C271" s="7"/>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="8"/>
       <c r="B272" s="8"/>
       <c r="C272" s="9"/>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="6"/>
       <c r="B273" s="6"/>
       <c r="C273" s="7"/>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="8"/>
       <c r="B274" s="8"/>
       <c r="C274" s="9"/>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="6"/>
       <c r="B275" s="6"/>
       <c r="C275" s="7"/>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="8"/>
       <c r="B276" s="8"/>
       <c r="C276" s="9"/>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="6"/>
       <c r="B277" s="6"/>
       <c r="C277" s="7"/>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="8"/>
       <c r="B278" s="8"/>
       <c r="C278" s="9"/>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="C279" s="7"/>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="8"/>
       <c r="B280" s="8"/>
       <c r="C280" s="9"/>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="6"/>
       <c r="B281" s="6"/>
       <c r="C281" s="7"/>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="8"/>
       <c r="B282" s="8"/>
       <c r="C282" s="9"/>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="6"/>
       <c r="B283" s="6"/>
       <c r="C283" s="7"/>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="8"/>
       <c r="B284" s="8"/>
       <c r="C284" s="9"/>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="6"/>
       <c r="B285" s="6"/>
       <c r="C285" s="7"/>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="8"/>
       <c r="B286" s="8"/>
       <c r="C286" s="9"/>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="6"/>
       <c r="B287" s="6"/>
       <c r="C287" s="7"/>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="8"/>
       <c r="B288" s="8"/>
       <c r="C288" s="9"/>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="6"/>
       <c r="B289" s="6"/>
       <c r="C289" s="7"/>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="8"/>
       <c r="B290" s="8"/>
       <c r="C290" s="9"/>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="6"/>
       <c r="B291" s="6"/>
       <c r="C291" s="7"/>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="8"/>
       <c r="B292" s="8"/>
       <c r="C292" s="9"/>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="6"/>
       <c r="B293" s="6"/>
       <c r="C293" s="7"/>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="8"/>
       <c r="B294" s="8"/>
       <c r="C294" s="9"/>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="6"/>
       <c r="B295" s="6"/>
       <c r="C295" s="7"/>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="8"/>
       <c r="B296" s="8"/>
       <c r="C296" s="9"/>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="6"/>
       <c r="B297" s="6"/>
       <c r="C297" s="7"/>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="8"/>
       <c r="B298" s="8"/>
       <c r="C298" s="9"/>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="6"/>
       <c r="B299" s="6"/>
       <c r="C299" s="7"/>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="8"/>
       <c r="B300" s="8"/>
       <c r="C300" s="9"/>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="6"/>
       <c r="B301" s="6"/>
       <c r="C301" s="7"/>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="8"/>
       <c r="B302" s="8"/>
       <c r="C302" s="9"/>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="6"/>
       <c r="B303" s="6"/>
       <c r="C303" s="7"/>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="8"/>
       <c r="B304" s="8"/>
       <c r="C304" s="9"/>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="6"/>
       <c r="B305" s="6"/>
       <c r="C305" s="7"/>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="8"/>
       <c r="B306" s="8"/>
       <c r="C306" s="9"/>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="6"/>
       <c r="B307" s="6"/>
       <c r="C307" s="7"/>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="8"/>
       <c r="B308" s="8"/>
       <c r="C308" s="9"/>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="6"/>
       <c r="B309" s="6"/>
       <c r="C309" s="7"/>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="8"/>
       <c r="B310" s="8"/>
       <c r="C310" s="9"/>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="6"/>
       <c r="B311" s="6"/>
       <c r="C311" s="7"/>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="8"/>
       <c r="B312" s="8"/>
       <c r="C312" s="9"/>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="6"/>
       <c r="B313" s="6"/>
       <c r="C313" s="7"/>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="8"/>
       <c r="B314" s="8"/>
       <c r="C314" s="9"/>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="6"/>
       <c r="B315" s="6"/>
       <c r="C315" s="7"/>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="8"/>
       <c r="B316" s="8"/>
       <c r="C316" s="9"/>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="6"/>
       <c r="B317" s="6"/>
       <c r="C317" s="7"/>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="8"/>
       <c r="B318" s="8"/>
       <c r="C318" s="9"/>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="6"/>
       <c r="B319" s="6"/>
       <c r="C319" s="7"/>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="8"/>
       <c r="B320" s="8"/>
       <c r="C320" s="9"/>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="6"/>
       <c r="B321" s="6"/>
       <c r="C321" s="7"/>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="8"/>
       <c r="B322" s="8"/>
       <c r="C322" s="9"/>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="6"/>
       <c r="B323" s="6"/>
       <c r="C323" s="7"/>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="8"/>
       <c r="B324" s="8"/>
       <c r="C324" s="9"/>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="6"/>
       <c r="B325" s="6"/>
       <c r="C325" s="7"/>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="8"/>
       <c r="B326" s="8"/>
       <c r="C326" s="9"/>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="6"/>
       <c r="B327" s="6"/>
       <c r="C327" s="7"/>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="8"/>
       <c r="B328" s="8"/>
       <c r="C328" s="9"/>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="6"/>
       <c r="B329" s="6"/>
       <c r="C329" s="7"/>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="8"/>
       <c r="B330" s="8"/>
       <c r="C330" s="9"/>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="6"/>
       <c r="B331" s="6"/>
       <c r="C331" s="7"/>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="8"/>
       <c r="B332" s="8"/>
       <c r="C332" s="9"/>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="6"/>
       <c r="B333" s="6"/>
       <c r="C333" s="7"/>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="8"/>
       <c r="B334" s="8"/>
       <c r="C334" s="9"/>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="6"/>
       <c r="B335" s="6"/>
       <c r="C335" s="7"/>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="8"/>
       <c r="B336" s="8"/>
       <c r="C336" s="9"/>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="6"/>
       <c r="B337" s="6"/>
       <c r="C337" s="7"/>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="8"/>
       <c r="B338" s="8"/>
       <c r="C338" s="9"/>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="6"/>
       <c r="B339" s="6"/>
       <c r="C339" s="7"/>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="8"/>
       <c r="B340" s="8"/>
       <c r="C340" s="9"/>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="6"/>
       <c r="B341" s="6"/>
       <c r="C341" s="7"/>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="8"/>
       <c r="B342" s="8"/>
       <c r="C342" s="9"/>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="6"/>
       <c r="B343" s="6"/>
       <c r="C343" s="7"/>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="8"/>
       <c r="B344" s="8"/>
       <c r="C344" s="9"/>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="6"/>
       <c r="B345" s="6"/>
       <c r="C345" s="7"/>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="8"/>
       <c r="B346" s="8"/>
       <c r="C346" s="9"/>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="6"/>
       <c r="B347" s="6"/>
       <c r="C347" s="7"/>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="8"/>
       <c r="B348" s="8"/>
       <c r="C348" s="9"/>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="6"/>
       <c r="B349" s="6"/>
       <c r="C349" s="7"/>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="8"/>
       <c r="B350" s="8"/>
       <c r="C350" s="9"/>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="6"/>
       <c r="B351" s="6"/>
       <c r="C351" s="7"/>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="8"/>
       <c r="B352" s="8"/>
       <c r="C352" s="9"/>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="6"/>
       <c r="B353" s="6"/>
       <c r="C353" s="7"/>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="8"/>
       <c r="B354" s="8"/>
       <c r="C354" s="9"/>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="6"/>
       <c r="B355" s="6"/>
       <c r="C355" s="7"/>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="8"/>
       <c r="B356" s="8"/>
       <c r="C356" s="9"/>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="6"/>
       <c r="B357" s="6"/>
       <c r="C357" s="7"/>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="8"/>
       <c r="B358" s="8"/>
       <c r="C358" s="9"/>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="6"/>
       <c r="B359" s="6"/>
       <c r="C359" s="7"/>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="8"/>
       <c r="B360" s="8"/>
       <c r="C360" s="9"/>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="6"/>
       <c r="B361" s="6"/>
       <c r="C361" s="7"/>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="8"/>
       <c r="B362" s="8"/>
       <c r="C362" s="9"/>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="6"/>
       <c r="B363" s="6"/>
       <c r="C363" s="7"/>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="8"/>
       <c r="B364" s="8"/>
       <c r="C364" s="9"/>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="6"/>
       <c r="B365" s="6"/>
       <c r="C365" s="7"/>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="8"/>
       <c r="B366" s="8"/>
       <c r="C366" s="9"/>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="6"/>
       <c r="B367" s="6"/>
       <c r="C367" s="7"/>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="8"/>
       <c r="B368" s="8"/>
       <c r="C368" s="9"/>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="6"/>
       <c r="B369" s="6"/>
       <c r="C369" s="7"/>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="8"/>
       <c r="B370" s="8"/>
       <c r="C370" s="9"/>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="6"/>
       <c r="B371" s="6"/>
       <c r="C371" s="7"/>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="8"/>
       <c r="B372" s="8"/>
       <c r="C372" s="9"/>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="6"/>
       <c r="B373" s="6"/>
       <c r="C373" s="7"/>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="8"/>
       <c r="B374" s="8"/>
       <c r="C374" s="9"/>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="6"/>
       <c r="B375" s="6"/>
       <c r="C375" s="7"/>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="8"/>
       <c r="B376" s="8"/>
       <c r="C376" s="9"/>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="6"/>
       <c r="B377" s="6"/>
       <c r="C377" s="7"/>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="8"/>
       <c r="B378" s="8"/>
       <c r="C378" s="9"/>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="6"/>
       <c r="B379" s="6"/>
       <c r="C379" s="7"/>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="8"/>
       <c r="B380" s="8"/>
       <c r="C380" s="9"/>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="6"/>
       <c r="B381" s="6"/>
       <c r="C381" s="7"/>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="8"/>
       <c r="B382" s="8"/>
       <c r="C382" s="9"/>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="6"/>
       <c r="B383" s="6"/>
       <c r="C383" s="7"/>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="8"/>
       <c r="B384" s="8"/>
       <c r="C384" s="9"/>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="6"/>
       <c r="B385" s="6"/>
       <c r="C385" s="7"/>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="8"/>
       <c r="B386" s="8"/>
       <c r="C386" s="9"/>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="6"/>
       <c r="B387" s="6"/>
       <c r="C387" s="7"/>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="8"/>
       <c r="B388" s="8"/>
       <c r="C388" s="9"/>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="6"/>
       <c r="B389" s="6"/>
       <c r="C389" s="7"/>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="8"/>
       <c r="B390" s="8"/>
       <c r="C390" s="9"/>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="6"/>
       <c r="B391" s="6"/>
       <c r="C391" s="7"/>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="8"/>
       <c r="B392" s="8"/>
       <c r="C392" s="9"/>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="6"/>
       <c r="B393" s="6"/>
       <c r="C393" s="7"/>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="8"/>
       <c r="B394" s="8"/>
       <c r="C394" s="9"/>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="6"/>
       <c r="B395" s="6"/>
       <c r="C395" s="7"/>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="8"/>
       <c r="B396" s="8"/>
       <c r="C396" s="9"/>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="6"/>
       <c r="B397" s="6"/>
       <c r="C397" s="7"/>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="8"/>
       <c r="B398" s="8"/>
       <c r="C398" s="9"/>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="6"/>
       <c r="B399" s="6"/>
       <c r="C399" s="7"/>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="8"/>
       <c r="B400" s="8"/>
       <c r="C400" s="9"/>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="6"/>
       <c r="B401" s="6"/>
       <c r="C401" s="7"/>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="8"/>
       <c r="B402" s="8"/>
       <c r="C402" s="9"/>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="6"/>
       <c r="B403" s="6"/>
       <c r="C403" s="7"/>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="8"/>
       <c r="B404" s="8"/>
       <c r="C404" s="9"/>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="6"/>
       <c r="B405" s="6"/>
       <c r="C405" s="7"/>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="8"/>
       <c r="B406" s="8"/>
       <c r="C406" s="9"/>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="6"/>
       <c r="B407" s="6"/>
       <c r="C407" s="7"/>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="8"/>
       <c r="B408" s="8"/>
       <c r="C408" s="9"/>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="6"/>
       <c r="B409" s="6"/>
       <c r="C409" s="7"/>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="8"/>
       <c r="B410" s="8"/>
       <c r="C410" s="9"/>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="6"/>
       <c r="B411" s="6"/>
       <c r="C411" s="7"/>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="8"/>
       <c r="B412" s="8"/>
       <c r="C412" s="9"/>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="6"/>
       <c r="B413" s="6"/>
       <c r="C413" s="7"/>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="8"/>
       <c r="B414" s="8"/>
       <c r="C414" s="9"/>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="6"/>
       <c r="B415" s="6"/>
       <c r="C415" s="7"/>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="8"/>
       <c r="B416" s="8"/>
       <c r="C416" s="9"/>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="6"/>
       <c r="B417" s="6"/>
       <c r="C417" s="7"/>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="8"/>
       <c r="B418" s="8"/>
       <c r="C418" s="9"/>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="6"/>
       <c r="B419" s="6"/>
       <c r="C419" s="7"/>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="8"/>
       <c r="B420" s="8"/>
       <c r="C420" s="9"/>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="6"/>
       <c r="B421" s="6"/>
       <c r="C421" s="7"/>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="8"/>
       <c r="B422" s="8"/>
       <c r="C422" s="9"/>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="6"/>
       <c r="B423" s="6"/>
       <c r="C423" s="7"/>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="8"/>
       <c r="B424" s="8"/>
       <c r="C424" s="9"/>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="6"/>
       <c r="B425" s="6"/>
       <c r="C425" s="7"/>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="8"/>
       <c r="B426" s="8"/>
       <c r="C426" s="9"/>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="6"/>
       <c r="B427" s="6"/>
       <c r="C427" s="7"/>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="8"/>
       <c r="B428" s="8"/>
       <c r="C428" s="9"/>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="6"/>
       <c r="B429" s="6"/>
       <c r="C429" s="7"/>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="8"/>
       <c r="B430" s="8"/>
       <c r="C430" s="9"/>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="6"/>
       <c r="B431" s="6"/>
       <c r="C431" s="7"/>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="8"/>
       <c r="B432" s="8"/>
       <c r="C432" s="9"/>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="6"/>
       <c r="B433" s="6"/>
       <c r="C433" s="7"/>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" s="8"/>
       <c r="B434" s="8"/>
       <c r="C434" s="9"/>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" s="6"/>
       <c r="B435" s="6"/>
       <c r="C435" s="7"/>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" s="8"/>
       <c r="B436" s="8"/>
       <c r="C436" s="9"/>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" s="6"/>
       <c r="B437" s="6"/>
       <c r="C437" s="7"/>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" s="8"/>
       <c r="B438" s="8"/>
       <c r="C438" s="9"/>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" s="6"/>
       <c r="B439" s="6"/>
       <c r="C439" s="7"/>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" s="8"/>
       <c r="B440" s="8"/>
       <c r="C440" s="9"/>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" s="6"/>
       <c r="B441" s="6"/>
       <c r="C441" s="7"/>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" s="8"/>
       <c r="B442" s="8"/>
       <c r="C442" s="9"/>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" s="6"/>
       <c r="B443" s="6"/>
       <c r="C443" s="7"/>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" s="8"/>
       <c r="B444" s="8"/>
       <c r="C444" s="9"/>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" s="6"/>
       <c r="B445" s="6"/>
       <c r="C445" s="7"/>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" s="8"/>
       <c r="B446" s="8"/>
       <c r="C446" s="9"/>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" s="6"/>
       <c r="B447" s="6"/>
       <c r="C447" s="7"/>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" s="8"/>
       <c r="B448" s="8"/>
       <c r="C448" s="9"/>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" s="6"/>
       <c r="B449" s="6"/>
       <c r="C449" s="7"/>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" s="8"/>
       <c r="B450" s="8"/>
       <c r="C450" s="9"/>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" s="6"/>
       <c r="B451" s="6"/>
       <c r="C451" s="7"/>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" s="8"/>
       <c r="B452" s="8"/>
       <c r="C452" s="9"/>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" s="6"/>
       <c r="B453" s="6"/>
       <c r="C453" s="7"/>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" s="8"/>
       <c r="B454" s="8"/>
       <c r="C454" s="9"/>
     </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" s="6"/>
       <c r="B455" s="6"/>
       <c r="C455" s="7"/>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" s="8"/>
       <c r="B456" s="8"/>
       <c r="C456" s="9"/>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" s="6"/>
       <c r="B457" s="6"/>
       <c r="C457" s="7"/>
     </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" s="8"/>
       <c r="B458" s="8"/>
       <c r="C458" s="9"/>
     </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" s="6"/>
       <c r="B459" s="6"/>
       <c r="C459" s="7"/>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" s="8"/>
       <c r="B460" s="8"/>
       <c r="C460" s="9"/>
     </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" s="6"/>
       <c r="B461" s="6"/>
       <c r="C461" s="7"/>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" s="8"/>
       <c r="B462" s="8"/>
       <c r="C462" s="9"/>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" s="6"/>
       <c r="B463" s="6"/>
       <c r="C463" s="7"/>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" s="8"/>
       <c r="B464" s="8"/>
       <c r="C464" s="9"/>
     </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" s="6"/>
       <c r="B465" s="6"/>
       <c r="C465" s="7"/>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" s="8"/>
       <c r="B466" s="8"/>
       <c r="C466" s="9"/>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" s="6"/>
       <c r="B467" s="6"/>
       <c r="C467" s="7"/>
     </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" s="8"/>
       <c r="B468" s="8"/>
       <c r="C468" s="9"/>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" s="6"/>
       <c r="B469" s="6"/>
       <c r="C469" s="7"/>
     </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" s="8"/>
       <c r="B470" s="8"/>
       <c r="C470" s="9"/>
     </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" s="6"/>
       <c r="B471" s="6"/>
       <c r="C471" s="7"/>
     </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" s="8"/>
       <c r="B472" s="8"/>
       <c r="C472" s="9"/>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" s="6"/>
       <c r="B473" s="6"/>
       <c r="C473" s="7"/>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" s="8"/>
       <c r="B474" s="8"/>
       <c r="C474" s="9"/>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" s="6"/>
       <c r="B475" s="6"/>
       <c r="C475" s="7"/>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" s="8"/>
       <c r="B476" s="8"/>
       <c r="C476" s="9"/>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" s="6"/>
       <c r="B477" s="6"/>
       <c r="C477" s="7"/>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" s="8"/>
       <c r="B478" s="8"/>
       <c r="C478" s="9"/>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" s="6"/>
       <c r="B479" s="6"/>
       <c r="C479" s="7"/>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" s="8"/>
       <c r="B480" s="8"/>
       <c r="C480" s="9"/>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" s="6"/>
       <c r="B481" s="6"/>
       <c r="C481" s="7"/>
     </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" s="8"/>
       <c r="B482" s="8"/>
       <c r="C482" s="9"/>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" s="6"/>
       <c r="B483" s="6"/>
       <c r="C483" s="7"/>
     </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" s="8"/>
       <c r="B484" s="8"/>
       <c r="C484" s="9"/>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" s="6"/>
       <c r="B485" s="6"/>
       <c r="C485" s="7"/>
     </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" s="8"/>
       <c r="B486" s="8"/>
       <c r="C486" s="9"/>
     </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" s="6"/>
       <c r="B487" s="6"/>
       <c r="C487" s="7"/>
     </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" s="8"/>
       <c r="B488" s="8"/>
       <c r="C488" s="9"/>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A489" s="6"/>
       <c r="B489" s="6"/>
       <c r="C489" s="7"/>
     </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" s="8"/>
       <c r="B490" s="8"/>
       <c r="C490" s="9"/>
     </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" s="6"/>
       <c r="B491" s="6"/>
       <c r="C491" s="7"/>
     </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A492" s="8"/>
       <c r="B492" s="8"/>
       <c r="C492" s="9"/>
     </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" s="6"/>
       <c r="B493" s="6"/>
       <c r="C493" s="7"/>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" s="8"/>
       <c r="B494" s="8"/>
       <c r="C494" s="9"/>
     </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A495" s="6"/>
       <c r="B495" s="6"/>
       <c r="C495" s="7"/>
     </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A496" s="8"/>
       <c r="B496" s="8"/>
       <c r="C496" s="9"/>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" s="6"/>
       <c r="B497" s="6"/>
       <c r="C497" s="7"/>
@@ -3228,32 +3252,32 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125"/>
-    <col min="2" max="2" width="20.54296875"/>
+    <col min="1" max="1" width="21.42578125"/>
+    <col min="2" max="2" width="20.5703125"/>
     <col min="3" max="3" width="23"/>
-    <col min="4" max="4" width="15.7265625"/>
-    <col min="5" max="1025" width="8.1796875"/>
+    <col min="4" max="4" width="15.7109375"/>
+    <col min="5" max="1025" width="8.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="12" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="12" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>10</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>12</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>7</v>
@@ -3266,9 +3290,9 @@
         <v>42578</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
@@ -3281,9 +3305,9 @@
         <v>42579</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>7</v>
@@ -3296,9 +3320,9 @@
         <v>42581</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
@@ -3311,9 +3335,9 @@
         <v>42585</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
@@ -3325,1465 +3349,1465 @@
         <v>42589</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" s="16" t="str">
         <f ca="1">IF(Completed!A7&lt;&gt;"", IF(Completed!D7="", TODAY(), Completed!D7), "")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" s="16" t="str">
         <f ca="1">IF(Completed!A8&lt;&gt;"", IF(Completed!D8="", TODAY(), Completed!D8), "")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" s="16" t="str">
         <f ca="1">IF(Completed!A9&lt;&gt;"", IF(Completed!D9="", TODAY(), Completed!D9), "")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="16" t="str">
         <f ca="1">IF(Completed!A10&lt;&gt;"", IF(Completed!D10="", TODAY(), Completed!D10), "")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" s="16" t="str">
         <f ca="1">IF(Completed!A11&lt;&gt;"", IF(Completed!D11="", TODAY(), Completed!D11), "")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="16" t="str">
         <f ca="1">IF(Completed!A12&lt;&gt;"", IF(Completed!D12="", TODAY(), Completed!D12), "")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" s="16" t="str">
         <f ca="1">IF(Completed!A13&lt;&gt;"", IF(Completed!D13="", TODAY(), Completed!D13), "")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="16" t="str">
         <f ca="1">IF(Completed!A14&lt;&gt;"", IF(Completed!D14="", TODAY(), Completed!D14), "")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="16" t="str">
         <f ca="1">IF(Completed!A15&lt;&gt;"", IF(Completed!D15="", TODAY(), Completed!D15), "")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" s="16" t="str">
         <f ca="1">IF(Completed!A16&lt;&gt;"", IF(Completed!D16="", TODAY(), Completed!D16), "")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="16" t="str">
         <f ca="1">IF(Completed!A17&lt;&gt;"", IF(Completed!D17="", TODAY(), Completed!D17), "")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="16" t="str">
         <f ca="1">IF(Completed!A18&lt;&gt;"", IF(Completed!D18="", TODAY(), Completed!D18), "")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="16" t="str">
         <f ca="1">IF(Completed!A19&lt;&gt;"", IF(Completed!D19="", TODAY(), Completed!D19), "")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="16" t="str">
         <f ca="1">IF(Completed!A20&lt;&gt;"", IF(Completed!D20="", TODAY(), Completed!D20), "")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="16" t="str">
         <f ca="1">IF(Completed!A21&lt;&gt;"", IF(Completed!D21="", TODAY(), Completed!D21), "")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="16" t="str">
         <f ca="1">IF(Completed!A22&lt;&gt;"", IF(Completed!D22="", TODAY(), Completed!D22), "")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="16" t="str">
         <f ca="1">IF(Completed!A23&lt;&gt;"", IF(Completed!D23="", TODAY(), Completed!D23), "")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="16" t="str">
         <f ca="1">IF(Completed!A24&lt;&gt;"", IF(Completed!D24="", TODAY(), Completed!D24), "")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="16" t="str">
         <f ca="1">IF(Completed!A25&lt;&gt;"", IF(Completed!D25="", TODAY(), Completed!D25), "")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="16" t="str">
         <f ca="1">IF(Completed!A26&lt;&gt;"", IF(Completed!D26="", TODAY(), Completed!D26), "")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="16" t="str">
         <f ca="1">IF(Completed!A27&lt;&gt;"", IF(Completed!D27="", TODAY(), Completed!D27), "")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="16" t="str">
         <f ca="1">IF(Completed!A28&lt;&gt;"", IF(Completed!D28="", TODAY(), Completed!D28), "")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="16" t="str">
         <f ca="1">IF(Completed!A29&lt;&gt;"", IF(Completed!D29="", TODAY(), Completed!D29), "")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="16" t="str">
         <f ca="1">IF(Completed!A30&lt;&gt;"", IF(Completed!D30="", TODAY(), Completed!D30), "")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="16" t="str">
         <f ca="1">IF(Completed!A31&lt;&gt;"", IF(Completed!D31="", TODAY(), Completed!D31), "")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="16" t="str">
         <f ca="1">IF(Completed!A32&lt;&gt;"", IF(Completed!D32="", TODAY(), Completed!D32), "")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="16" t="str">
         <f ca="1">IF(Completed!A33&lt;&gt;"", IF(Completed!D33="", TODAY(), Completed!D33), "")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="16" t="str">
         <f ca="1">IF(Completed!A34&lt;&gt;"", IF(Completed!D34="", TODAY(), Completed!D34), "")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="16" t="str">
         <f ca="1">IF(Completed!A35&lt;&gt;"", IF(Completed!D35="", TODAY(), Completed!D35), "")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="16" t="str">
         <f ca="1">IF(Completed!A36&lt;&gt;"", IF(Completed!D36="", TODAY(), Completed!D36), "")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="16" t="str">
         <f ca="1">IF(Completed!A37&lt;&gt;"", IF(Completed!D37="", TODAY(), Completed!D37), "")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="str">
         <f ca="1">IF(Completed!A38&lt;&gt;"", IF(Completed!D38="", TODAY(), Completed!D38), "")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="str">
         <f ca="1">IF(Completed!A39&lt;&gt;"", IF(Completed!D39="", TODAY(), Completed!D39), "")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="16" t="str">
         <f ca="1">IF(Completed!A40&lt;&gt;"", IF(Completed!D40="", TODAY(), Completed!D40), "")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="str">
         <f ca="1">IF(Completed!A41&lt;&gt;"", IF(Completed!D41="", TODAY(), Completed!D41), "")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="16" t="str">
         <f ca="1">IF(Completed!A42&lt;&gt;"", IF(Completed!D42="", TODAY(), Completed!D42), "")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="16" t="str">
         <f ca="1">IF(Completed!A43&lt;&gt;"", IF(Completed!D43="", TODAY(), Completed!D43), "")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="16" t="str">
         <f ca="1">IF(Completed!A44&lt;&gt;"", IF(Completed!D44="", TODAY(), Completed!D44), "")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="16" t="str">
         <f ca="1">IF(Completed!A45&lt;&gt;"", IF(Completed!D45="", TODAY(), Completed!D45), "")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="16" t="str">
         <f ca="1">IF(Completed!A46&lt;&gt;"", IF(Completed!D46="", TODAY(), Completed!D46), "")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="16" t="str">
         <f ca="1">IF(Completed!A47&lt;&gt;"", IF(Completed!D47="", TODAY(), Completed!D47), "")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="16" t="str">
         <f ca="1">IF(Completed!A48&lt;&gt;"", IF(Completed!D48="", TODAY(), Completed!D48), "")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="16" t="str">
         <f ca="1">IF(Completed!A49&lt;&gt;"", IF(Completed!D49="", TODAY(), Completed!D49), "")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="16" t="str">
         <f ca="1">IF(Completed!A50&lt;&gt;"", IF(Completed!D50="", TODAY(), Completed!D50), "")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="16" t="str">
         <f ca="1">IF(Completed!A51&lt;&gt;"", IF(Completed!D51="", TODAY(), Completed!D51), "")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="16" t="str">
         <f ca="1">IF(Completed!A52&lt;&gt;"", IF(Completed!D52="", TODAY(), Completed!D52), "")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="16" t="str">
         <f ca="1">IF(Completed!A53&lt;&gt;"", IF(Completed!D53="", TODAY(), Completed!D53), "")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="16" t="str">
         <f ca="1">IF(Completed!A54&lt;&gt;"", IF(Completed!D54="", TODAY(), Completed!D54), "")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="16" t="str">
         <f ca="1">IF(Completed!A55&lt;&gt;"", IF(Completed!D55="", TODAY(), Completed!D55), "")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="16" t="str">
         <f ca="1">IF(Completed!A56&lt;&gt;"", IF(Completed!D56="", TODAY(), Completed!D56), "")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="16" t="str">
         <f ca="1">IF(Completed!A57&lt;&gt;"", IF(Completed!D57="", TODAY(), Completed!D57), "")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="16" t="str">
         <f ca="1">IF(Completed!A58&lt;&gt;"", IF(Completed!D58="", TODAY(), Completed!D58), "")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="16" t="str">
         <f ca="1">IF(Completed!A59&lt;&gt;"", IF(Completed!D59="", TODAY(), Completed!D59), "")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="16" t="str">
         <f ca="1">IF(Completed!A60&lt;&gt;"", IF(Completed!D60="", TODAY(), Completed!D60), "")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="16" t="str">
         <f ca="1">IF(Completed!A61&lt;&gt;"", IF(Completed!D61="", TODAY(), Completed!D61), "")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="16" t="str">
         <f ca="1">IF(Completed!A62&lt;&gt;"", IF(Completed!D62="", TODAY(), Completed!D62), "")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="16" t="str">
         <f ca="1">IF(Completed!A63&lt;&gt;"", IF(Completed!D63="", TODAY(), Completed!D63), "")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="16" t="str">
         <f ca="1">IF(Completed!A64&lt;&gt;"", IF(Completed!D64="", TODAY(), Completed!D64), "")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="16" t="str">
         <f ca="1">IF(Completed!A65&lt;&gt;"", IF(Completed!D65="", TODAY(), Completed!D65), "")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="16" t="str">
         <f ca="1">IF(Completed!A66&lt;&gt;"", IF(Completed!D66="", TODAY(), Completed!D66), "")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="16" t="str">
         <f ca="1">IF(Completed!A67&lt;&gt;"", IF(Completed!D67="", TODAY(), Completed!D67), "")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="16" t="str">
         <f ca="1">IF(Completed!A68&lt;&gt;"", IF(Completed!D68="", TODAY(), Completed!D68), "")</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="16" t="str">
         <f ca="1">IF(Completed!A69&lt;&gt;"", IF(Completed!D69="", TODAY(), Completed!D69), "")</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="16" t="str">
         <f ca="1">IF(Completed!A70&lt;&gt;"", IF(Completed!D70="", TODAY(), Completed!D70), "")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="16" t="str">
         <f ca="1">IF(Completed!A71&lt;&gt;"", IF(Completed!D71="", TODAY(), Completed!D71), "")</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="16" t="str">
         <f ca="1">IF(Completed!A72&lt;&gt;"", IF(Completed!D72="", TODAY(), Completed!D72), "")</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="16" t="str">
         <f ca="1">IF(Completed!A73&lt;&gt;"", IF(Completed!D73="", TODAY(), Completed!D73), "")</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="16" t="str">
         <f ca="1">IF(Completed!A74&lt;&gt;"", IF(Completed!D74="", TODAY(), Completed!D74), "")</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="16" t="str">
         <f ca="1">IF(Completed!A75&lt;&gt;"", IF(Completed!D75="", TODAY(), Completed!D75), "")</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="16" t="str">
         <f ca="1">IF(Completed!A76&lt;&gt;"", IF(Completed!D76="", TODAY(), Completed!D76), "")</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="16" t="str">
         <f ca="1">IF(Completed!A77&lt;&gt;"", IF(Completed!D77="", TODAY(), Completed!D77), "")</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="16" t="str">
         <f ca="1">IF(Completed!A78&lt;&gt;"", IF(Completed!D78="", TODAY(), Completed!D78), "")</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="16" t="str">
         <f ca="1">IF(Completed!A79&lt;&gt;"", IF(Completed!D79="", TODAY(), Completed!D79), "")</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="16" t="str">
         <f ca="1">IF(Completed!A80&lt;&gt;"", IF(Completed!D80="", TODAY(), Completed!D80), "")</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="16" t="str">
         <f ca="1">IF(Completed!A81&lt;&gt;"", IF(Completed!D81="", TODAY(), Completed!D81), "")</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="16" t="str">
         <f ca="1">IF(Completed!A82&lt;&gt;"", IF(Completed!D82="", TODAY(), Completed!D82), "")</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="16" t="str">
         <f ca="1">IF(Completed!A83&lt;&gt;"", IF(Completed!D83="", TODAY(), Completed!D83), "")</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="16" t="str">
         <f ca="1">IF(Completed!A84&lt;&gt;"", IF(Completed!D84="", TODAY(), Completed!D84), "")</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="16" t="str">
         <f ca="1">IF(Completed!A85&lt;&gt;"", IF(Completed!D85="", TODAY(), Completed!D85), "")</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="16" t="str">
         <f ca="1">IF(Completed!A86&lt;&gt;"", IF(Completed!D86="", TODAY(), Completed!D86), "")</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="16" t="str">
         <f ca="1">IF(Completed!A87&lt;&gt;"", IF(Completed!D87="", TODAY(), Completed!D87), "")</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="16" t="str">
         <f ca="1">IF(Completed!A88&lt;&gt;"", IF(Completed!D88="", TODAY(), Completed!D88), "")</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="16" t="str">
         <f ca="1">IF(Completed!A89&lt;&gt;"", IF(Completed!D89="", TODAY(), Completed!D89), "")</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="16" t="str">
         <f ca="1">IF(Completed!A90&lt;&gt;"", IF(Completed!D90="", TODAY(), Completed!D90), "")</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="16" t="str">
         <f ca="1">IF(Completed!A91&lt;&gt;"", IF(Completed!D91="", TODAY(), Completed!D91), "")</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="16" t="str">
         <f ca="1">IF(Completed!A92&lt;&gt;"", IF(Completed!D92="", TODAY(), Completed!D92), "")</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="16" t="str">
         <f ca="1">IF(Completed!A93&lt;&gt;"", IF(Completed!D93="", TODAY(), Completed!D93), "")</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="16" t="str">
         <f ca="1">IF(Completed!A94&lt;&gt;"", IF(Completed!D94="", TODAY(), Completed!D94), "")</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="16" t="str">
         <f ca="1">IF(Completed!A95&lt;&gt;"", IF(Completed!D95="", TODAY(), Completed!D95), "")</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="16" t="str">
         <f ca="1">IF(Completed!A96&lt;&gt;"", IF(Completed!D96="", TODAY(), Completed!D96), "")</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="16" t="str">
         <f ca="1">IF(Completed!A97&lt;&gt;"", IF(Completed!D97="", TODAY(), Completed!D97), "")</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="16" t="str">
         <f ca="1">IF(Completed!A98&lt;&gt;"", IF(Completed!D98="", TODAY(), Completed!D98), "")</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="16" t="str">
         <f ca="1">IF(Completed!A99&lt;&gt;"", IF(Completed!D99="", TODAY(), Completed!D99), "")</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="16" t="str">
         <f ca="1">IF(Completed!A100&lt;&gt;"", IF(Completed!D100="", TODAY(), Completed!D100), "")</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="16" t="str">
         <f ca="1">IF(Completed!A101&lt;&gt;"", IF(Completed!D101="", TODAY(), Completed!D101), "")</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="16" t="str">
         <f ca="1">IF(Completed!A102&lt;&gt;"", IF(Completed!D102="", TODAY(), Completed!D102), "")</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D103" s="16" t="str">
         <f ca="1">IF(Completed!A103&lt;&gt;"", IF(Completed!D103="", TODAY(), Completed!D103), "")</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="16" t="str">
         <f ca="1">IF(Completed!A104&lt;&gt;"", IF(Completed!D104="", TODAY(), Completed!D104), "")</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105" s="16" t="str">
         <f ca="1">IF(Completed!A105&lt;&gt;"", IF(Completed!D105="", TODAY(), Completed!D105), "")</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D106" s="16" t="str">
         <f ca="1">IF(Completed!A106&lt;&gt;"", IF(Completed!D106="", TODAY(), Completed!D106), "")</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107" s="16" t="str">
         <f ca="1">IF(Completed!A107&lt;&gt;"", IF(Completed!D107="", TODAY(), Completed!D107), "")</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="16" t="str">
         <f ca="1">IF(Completed!A108&lt;&gt;"", IF(Completed!D108="", TODAY(), Completed!D108), "")</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D109" s="16" t="str">
         <f ca="1">IF(Completed!A109&lt;&gt;"", IF(Completed!D109="", TODAY(), Completed!D109), "")</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="16" t="str">
         <f ca="1">IF(Completed!A110&lt;&gt;"", IF(Completed!D110="", TODAY(), Completed!D110), "")</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111" s="16" t="str">
         <f ca="1">IF(Completed!A111&lt;&gt;"", IF(Completed!D111="", TODAY(), Completed!D111), "")</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112" s="16" t="str">
         <f ca="1">IF(Completed!A112&lt;&gt;"", IF(Completed!D112="", TODAY(), Completed!D112), "")</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="16" t="str">
         <f ca="1">IF(Completed!A113&lt;&gt;"", IF(Completed!D113="", TODAY(), Completed!D113), "")</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="16" t="str">
         <f ca="1">IF(Completed!A114&lt;&gt;"", IF(Completed!D114="", TODAY(), Completed!D114), "")</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115" s="16" t="str">
         <f ca="1">IF(Completed!A115&lt;&gt;"", IF(Completed!D115="", TODAY(), Completed!D115), "")</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="16" t="str">
         <f ca="1">IF(Completed!A116&lt;&gt;"", IF(Completed!D116="", TODAY(), Completed!D116), "")</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D117" s="16" t="str">
         <f ca="1">IF(Completed!A117&lt;&gt;"", IF(Completed!D117="", TODAY(), Completed!D117), "")</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118" s="16" t="str">
         <f ca="1">IF(Completed!A118&lt;&gt;"", IF(Completed!D118="", TODAY(), Completed!D118), "")</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119" s="16" t="str">
         <f ca="1">IF(Completed!A119&lt;&gt;"", IF(Completed!D119="", TODAY(), Completed!D119), "")</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120" s="16" t="str">
         <f ca="1">IF(Completed!A120&lt;&gt;"", IF(Completed!D120="", TODAY(), Completed!D120), "")</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121" s="16" t="str">
         <f ca="1">IF(Completed!A121&lt;&gt;"", IF(Completed!D121="", TODAY(), Completed!D121), "")</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122" s="16" t="str">
         <f ca="1">IF(Completed!A122&lt;&gt;"", IF(Completed!D122="", TODAY(), Completed!D122), "")</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="16" t="str">
         <f ca="1">IF(Completed!A123&lt;&gt;"", IF(Completed!D123="", TODAY(), Completed!D123), "")</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="16" t="str">
         <f ca="1">IF(Completed!A124&lt;&gt;"", IF(Completed!D124="", TODAY(), Completed!D124), "")</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D125" s="16" t="str">
         <f ca="1">IF(Completed!A125&lt;&gt;"", IF(Completed!D125="", TODAY(), Completed!D125), "")</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D126" s="16" t="str">
         <f ca="1">IF(Completed!A126&lt;&gt;"", IF(Completed!D126="", TODAY(), Completed!D126), "")</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D127" s="16" t="str">
         <f ca="1">IF(Completed!A127&lt;&gt;"", IF(Completed!D127="", TODAY(), Completed!D127), "")</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D128" s="16" t="str">
         <f ca="1">IF(Completed!A128&lt;&gt;"", IF(Completed!D128="", TODAY(), Completed!D128), "")</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129" s="16" t="str">
         <f ca="1">IF(Completed!A129&lt;&gt;"", IF(Completed!D129="", TODAY(), Completed!D129), "")</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130" s="16" t="str">
         <f ca="1">IF(Completed!A130&lt;&gt;"", IF(Completed!D130="", TODAY(), Completed!D130), "")</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131" s="16" t="str">
         <f ca="1">IF(Completed!A131&lt;&gt;"", IF(Completed!D131="", TODAY(), Completed!D131), "")</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132" s="16" t="str">
         <f ca="1">IF(Completed!A132&lt;&gt;"", IF(Completed!D132="", TODAY(), Completed!D132), "")</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133" s="16" t="str">
         <f ca="1">IF(Completed!A133&lt;&gt;"", IF(Completed!D133="", TODAY(), Completed!D133), "")</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D134" s="16" t="str">
         <f ca="1">IF(Completed!A134&lt;&gt;"", IF(Completed!D134="", TODAY(), Completed!D134), "")</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D135" s="16" t="str">
         <f ca="1">IF(Completed!A135&lt;&gt;"", IF(Completed!D135="", TODAY(), Completed!D135), "")</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" s="16" t="str">
         <f ca="1">IF(Completed!A136&lt;&gt;"", IF(Completed!D136="", TODAY(), Completed!D136), "")</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137" s="16" t="str">
         <f ca="1">IF(Completed!A137&lt;&gt;"", IF(Completed!D137="", TODAY(), Completed!D137), "")</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D138" s="16" t="str">
         <f ca="1">IF(Completed!A138&lt;&gt;"", IF(Completed!D138="", TODAY(), Completed!D138), "")</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D139" s="16" t="str">
         <f ca="1">IF(Completed!A139&lt;&gt;"", IF(Completed!D139="", TODAY(), Completed!D139), "")</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D140" s="16" t="str">
         <f ca="1">IF(Completed!A140&lt;&gt;"", IF(Completed!D140="", TODAY(), Completed!D140), "")</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D141" s="16" t="str">
         <f ca="1">IF(Completed!A141&lt;&gt;"", IF(Completed!D141="", TODAY(), Completed!D141), "")</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D142" s="16" t="str">
         <f ca="1">IF(Completed!A142&lt;&gt;"", IF(Completed!D142="", TODAY(), Completed!D142), "")</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D143" s="16" t="str">
         <f ca="1">IF(Completed!A143&lt;&gt;"", IF(Completed!D143="", TODAY(), Completed!D143), "")</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D144" s="16" t="str">
         <f ca="1">IF(Completed!A144&lt;&gt;"", IF(Completed!D144="", TODAY(), Completed!D144), "")</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D145" s="16" t="str">
         <f ca="1">IF(Completed!A145&lt;&gt;"", IF(Completed!D145="", TODAY(), Completed!D145), "")</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D146" s="16" t="str">
         <f ca="1">IF(Completed!A146&lt;&gt;"", IF(Completed!D146="", TODAY(), Completed!D146), "")</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147" s="16" t="str">
         <f ca="1">IF(Completed!A147&lt;&gt;"", IF(Completed!D147="", TODAY(), Completed!D147), "")</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148" s="16" t="str">
         <f ca="1">IF(Completed!A148&lt;&gt;"", IF(Completed!D148="", TODAY(), Completed!D148), "")</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D149" s="16" t="str">
         <f ca="1">IF(Completed!A149&lt;&gt;"", IF(Completed!D149="", TODAY(), Completed!D149), "")</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D150" s="16" t="str">
         <f ca="1">IF(Completed!A150&lt;&gt;"", IF(Completed!D150="", TODAY(), Completed!D150), "")</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D151" s="16" t="str">
         <f ca="1">IF(Completed!A151&lt;&gt;"", IF(Completed!D151="", TODAY(), Completed!D151), "")</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D152" s="16" t="str">
         <f ca="1">IF(Completed!A152&lt;&gt;"", IF(Completed!D152="", TODAY(), Completed!D152), "")</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D153" s="16" t="str">
         <f ca="1">IF(Completed!A153&lt;&gt;"", IF(Completed!D153="", TODAY(), Completed!D153), "")</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D154" s="16" t="str">
         <f ca="1">IF(Completed!A154&lt;&gt;"", IF(Completed!D154="", TODAY(), Completed!D154), "")</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D155" s="16" t="str">
         <f ca="1">IF(Completed!A155&lt;&gt;"", IF(Completed!D155="", TODAY(), Completed!D155), "")</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D156" s="16" t="str">
         <f ca="1">IF(Completed!A156&lt;&gt;"", IF(Completed!D156="", TODAY(), Completed!D156), "")</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D157" s="16" t="str">
         <f ca="1">IF(Completed!A157&lt;&gt;"", IF(Completed!D157="", TODAY(), Completed!D157), "")</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D158" s="16" t="str">
         <f ca="1">IF(Completed!A158&lt;&gt;"", IF(Completed!D158="", TODAY(), Completed!D158), "")</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D159" s="16" t="str">
         <f ca="1">IF(Completed!A159&lt;&gt;"", IF(Completed!D159="", TODAY(), Completed!D159), "")</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D160" s="16" t="str">
         <f ca="1">IF(Completed!A160&lt;&gt;"", IF(Completed!D160="", TODAY(), Completed!D160), "")</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D161" s="16" t="str">
         <f ca="1">IF(Completed!A161&lt;&gt;"", IF(Completed!D161="", TODAY(), Completed!D161), "")</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D162" s="16" t="str">
         <f ca="1">IF(Completed!A162&lt;&gt;"", IF(Completed!D162="", TODAY(), Completed!D162), "")</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D163" s="16" t="str">
         <f ca="1">IF(Completed!A163&lt;&gt;"", IF(Completed!D163="", TODAY(), Completed!D163), "")</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D164" s="16" t="str">
         <f ca="1">IF(Completed!A164&lt;&gt;"", IF(Completed!D164="", TODAY(), Completed!D164), "")</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D165" s="16" t="str">
         <f ca="1">IF(Completed!A165&lt;&gt;"", IF(Completed!D165="", TODAY(), Completed!D165), "")</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D166" s="16" t="str">
         <f ca="1">IF(Completed!A166&lt;&gt;"", IF(Completed!D166="", TODAY(), Completed!D166), "")</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D167" s="16" t="str">
         <f ca="1">IF(Completed!A167&lt;&gt;"", IF(Completed!D167="", TODAY(), Completed!D167), "")</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D168" s="16" t="str">
         <f ca="1">IF(Completed!A168&lt;&gt;"", IF(Completed!D168="", TODAY(), Completed!D168), "")</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D169" s="16" t="str">
         <f ca="1">IF(Completed!A169&lt;&gt;"", IF(Completed!D169="", TODAY(), Completed!D169), "")</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D170" s="16" t="str">
         <f ca="1">IF(Completed!A170&lt;&gt;"", IF(Completed!D170="", TODAY(), Completed!D170), "")</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D171" s="16" t="str">
         <f ca="1">IF(Completed!A171&lt;&gt;"", IF(Completed!D171="", TODAY(), Completed!D171), "")</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D172" s="16" t="str">
         <f ca="1">IF(Completed!A172&lt;&gt;"", IF(Completed!D172="", TODAY(), Completed!D172), "")</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D173" s="16" t="str">
         <f ca="1">IF(Completed!A173&lt;&gt;"", IF(Completed!D173="", TODAY(), Completed!D173), "")</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D174" s="16" t="str">
         <f ca="1">IF(Completed!A174&lt;&gt;"", IF(Completed!D174="", TODAY(), Completed!D174), "")</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D175" s="16" t="str">
         <f ca="1">IF(Completed!A175&lt;&gt;"", IF(Completed!D175="", TODAY(), Completed!D175), "")</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D176" s="16" t="str">
         <f ca="1">IF(Completed!A176&lt;&gt;"", IF(Completed!D176="", TODAY(), Completed!D176), "")</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D177" s="16" t="str">
         <f ca="1">IF(Completed!A177&lt;&gt;"", IF(Completed!D177="", TODAY(), Completed!D177), "")</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D178" s="16" t="str">
         <f ca="1">IF(Completed!A178&lt;&gt;"", IF(Completed!D178="", TODAY(), Completed!D178), "")</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D179" s="16" t="str">
         <f ca="1">IF(Completed!A179&lt;&gt;"", IF(Completed!D179="", TODAY(), Completed!D179), "")</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D180" s="16" t="str">
         <f ca="1">IF(Completed!A180&lt;&gt;"", IF(Completed!D180="", TODAY(), Completed!D180), "")</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D181" s="16" t="str">
         <f ca="1">IF(Completed!A181&lt;&gt;"", IF(Completed!D181="", TODAY(), Completed!D181), "")</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D182" s="16" t="str">
         <f ca="1">IF(Completed!A182&lt;&gt;"", IF(Completed!D182="", TODAY(), Completed!D182), "")</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D183" s="16" t="str">
         <f ca="1">IF(Completed!A183&lt;&gt;"", IF(Completed!D183="", TODAY(), Completed!D183), "")</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D184" s="16" t="str">
         <f ca="1">IF(Completed!A184&lt;&gt;"", IF(Completed!D184="", TODAY(), Completed!D184), "")</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D185" s="16" t="str">
         <f ca="1">IF(Completed!A185&lt;&gt;"", IF(Completed!D185="", TODAY(), Completed!D185), "")</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D186" s="16" t="str">
         <f ca="1">IF(Completed!A186&lt;&gt;"", IF(Completed!D186="", TODAY(), Completed!D186), "")</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D187" s="16" t="str">
         <f ca="1">IF(Completed!A187&lt;&gt;"", IF(Completed!D187="", TODAY(), Completed!D187), "")</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D188" s="16" t="str">
         <f ca="1">IF(Completed!A188&lt;&gt;"", IF(Completed!D188="", TODAY(), Completed!D188), "")</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D189" s="16" t="str">
         <f ca="1">IF(Completed!A189&lt;&gt;"", IF(Completed!D189="", TODAY(), Completed!D189), "")</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D190" s="16" t="str">
         <f ca="1">IF(Completed!A190&lt;&gt;"", IF(Completed!D190="", TODAY(), Completed!D190), "")</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D191" s="16" t="str">
         <f ca="1">IF(Completed!A191&lt;&gt;"", IF(Completed!D191="", TODAY(), Completed!D191), "")</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D192" s="16" t="str">
         <f ca="1">IF(Completed!A192&lt;&gt;"", IF(Completed!D192="", TODAY(), Completed!D192), "")</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D193" s="16" t="str">
         <f ca="1">IF(Completed!A193&lt;&gt;"", IF(Completed!D193="", TODAY(), Completed!D193), "")</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D194" s="16" t="str">
         <f ca="1">IF(Completed!A194&lt;&gt;"", IF(Completed!D194="", TODAY(), Completed!D194), "")</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D195" s="16" t="str">
         <f ca="1">IF(Completed!A195&lt;&gt;"", IF(Completed!D195="", TODAY(), Completed!D195), "")</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D196" s="16" t="str">
         <f ca="1">IF(Completed!A196&lt;&gt;"", IF(Completed!D196="", TODAY(), Completed!D196), "")</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D197" s="16" t="str">
         <f ca="1">IF(Completed!A197&lt;&gt;"", IF(Completed!D197="", TODAY(), Completed!D197), "")</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D198" s="16" t="str">
         <f ca="1">IF(Completed!A198&lt;&gt;"", IF(Completed!D198="", TODAY(), Completed!D198), "")</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D199" s="16" t="str">
         <f ca="1">IF(Completed!A199&lt;&gt;"", IF(Completed!D199="", TODAY(), Completed!D199), "")</f>
         <v/>
       </c>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D200" s="16" t="str">
         <f ca="1">IF(Completed!A200&lt;&gt;"", IF(Completed!D200="", TODAY(), Completed!D200), "")</f>
         <v/>
       </c>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D201" s="16" t="str">
         <f ca="1">IF(Completed!A201&lt;&gt;"", IF(Completed!D201="", TODAY(), Completed!D201), "")</f>
         <v/>
       </c>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D202" s="16" t="str">
         <f ca="1">IF(Completed!A202&lt;&gt;"", IF(Completed!D202="", TODAY(), Completed!D202), "")</f>
         <v/>
       </c>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D203" s="16" t="str">
         <f ca="1">IF(Completed!A203&lt;&gt;"", IF(Completed!D203="", TODAY(), Completed!D203), "")</f>
         <v/>
       </c>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D204" s="16" t="str">
         <f ca="1">IF(Completed!A204&lt;&gt;"", IF(Completed!D204="", TODAY(), Completed!D204), "")</f>
         <v/>
       </c>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D205" s="16" t="str">
         <f ca="1">IF(Completed!A205&lt;&gt;"", IF(Completed!D205="", TODAY(), Completed!D205), "")</f>
         <v/>
       </c>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D206" s="16" t="str">
         <f ca="1">IF(Completed!A206&lt;&gt;"", IF(Completed!D206="", TODAY(), Completed!D206), "")</f>
         <v/>
       </c>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D207" s="16" t="str">
         <f ca="1">IF(Completed!A207&lt;&gt;"", IF(Completed!D207="", TODAY(), Completed!D207), "")</f>
         <v/>
       </c>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D208" s="16" t="str">
         <f ca="1">IF(Completed!A208&lt;&gt;"", IF(Completed!D208="", TODAY(), Completed!D208), "")</f>
         <v/>
       </c>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D209" s="16" t="str">
         <f ca="1">IF(Completed!A209&lt;&gt;"", IF(Completed!D209="", TODAY(), Completed!D209), "")</f>
         <v/>
       </c>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D210" s="16" t="str">
         <f ca="1">IF(Completed!A210&lt;&gt;"", IF(Completed!D210="", TODAY(), Completed!D210), "")</f>
         <v/>
       </c>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D211" s="16" t="str">
         <f ca="1">IF(Completed!A211&lt;&gt;"", IF(Completed!D211="", TODAY(), Completed!D211), "")</f>
         <v/>
       </c>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D212" s="16" t="str">
         <f ca="1">IF(Completed!A212&lt;&gt;"", IF(Completed!D212="", TODAY(), Completed!D212), "")</f>
         <v/>
       </c>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D213" s="16" t="str">
         <f ca="1">IF(Completed!A213&lt;&gt;"", IF(Completed!D213="", TODAY(), Completed!D213), "")</f>
         <v/>
       </c>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D214" s="16" t="str">
         <f ca="1">IF(Completed!A214&lt;&gt;"", IF(Completed!D214="", TODAY(), Completed!D214), "")</f>
         <v/>
       </c>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D215" s="16" t="str">
         <f ca="1">IF(Completed!A215&lt;&gt;"", IF(Completed!D215="", TODAY(), Completed!D215), "")</f>
         <v/>
       </c>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D216" s="16" t="str">
         <f ca="1">IF(Completed!A216&lt;&gt;"", IF(Completed!D216="", TODAY(), Completed!D216), "")</f>
         <v/>
       </c>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D217" s="16" t="str">
         <f ca="1">IF(Completed!A217&lt;&gt;"", IF(Completed!D217="", TODAY(), Completed!D217), "")</f>
         <v/>
       </c>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D218" s="16" t="str">
         <f ca="1">IF(Completed!A218&lt;&gt;"", IF(Completed!D218="", TODAY(), Completed!D218), "")</f>
         <v/>
       </c>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D219" s="16" t="str">
         <f ca="1">IF(Completed!A219&lt;&gt;"", IF(Completed!D219="", TODAY(), Completed!D219), "")</f>
         <v/>
       </c>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D220" s="16" t="str">
         <f ca="1">IF(Completed!A220&lt;&gt;"", IF(Completed!D220="", TODAY(), Completed!D220), "")</f>
         <v/>
       </c>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D221" s="16" t="str">
         <f ca="1">IF(Completed!A221&lt;&gt;"", IF(Completed!D221="", TODAY(), Completed!D221), "")</f>
         <v/>
       </c>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D222" s="16" t="str">
         <f ca="1">IF(Completed!A222&lt;&gt;"", IF(Completed!D222="", TODAY(), Completed!D222), "")</f>
         <v/>
       </c>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D223" s="16" t="str">
         <f ca="1">IF(Completed!A223&lt;&gt;"", IF(Completed!D223="", TODAY(), Completed!D223), "")</f>
         <v/>
       </c>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D224" s="16" t="str">
         <f ca="1">IF(Completed!A224&lt;&gt;"", IF(Completed!D224="", TODAY(), Completed!D224), "")</f>
         <v/>
       </c>
     </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D225" s="16" t="str">
         <f ca="1">IF(Completed!A225&lt;&gt;"", IF(Completed!D225="", TODAY(), Completed!D225), "")</f>
         <v/>
       </c>
     </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D226" s="16" t="str">
         <f ca="1">IF(Completed!A226&lt;&gt;"", IF(Completed!D226="", TODAY(), Completed!D226), "")</f>
         <v/>
       </c>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D227" s="16" t="str">
         <f ca="1">IF(Completed!A227&lt;&gt;"", IF(Completed!D227="", TODAY(), Completed!D227), "")</f>
         <v/>
       </c>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D228" s="16" t="str">
         <f ca="1">IF(Completed!A228&lt;&gt;"", IF(Completed!D228="", TODAY(), Completed!D228), "")</f>
         <v/>
       </c>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D229" s="16" t="str">
         <f ca="1">IF(Completed!A229&lt;&gt;"", IF(Completed!D229="", TODAY(), Completed!D229), "")</f>
         <v/>
       </c>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D230" s="16" t="str">
         <f ca="1">IF(Completed!A230&lt;&gt;"", IF(Completed!D230="", TODAY(), Completed!D230), "")</f>
         <v/>
       </c>
     </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D231" s="16" t="str">
         <f ca="1">IF(Completed!A231&lt;&gt;"", IF(Completed!D231="", TODAY(), Completed!D231), "")</f>
         <v/>
       </c>
     </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D232" s="16" t="str">
         <f ca="1">IF(Completed!A232&lt;&gt;"", IF(Completed!D232="", TODAY(), Completed!D232), "")</f>
         <v/>
       </c>
     </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D233" s="16" t="str">
         <f ca="1">IF(Completed!A233&lt;&gt;"", IF(Completed!D233="", TODAY(), Completed!D233), "")</f>
         <v/>
       </c>
     </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D234" s="16" t="str">
         <f ca="1">IF(Completed!A234&lt;&gt;"", IF(Completed!D234="", TODAY(), Completed!D234), "")</f>
         <v/>
       </c>
     </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D235" s="16" t="str">
         <f ca="1">IF(Completed!A235&lt;&gt;"", IF(Completed!D235="", TODAY(), Completed!D235), "")</f>
         <v/>
       </c>
     </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D236" s="16" t="str">
         <f ca="1">IF(Completed!A236&lt;&gt;"", IF(Completed!D236="", TODAY(), Completed!D236), "")</f>
         <v/>
       </c>
     </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D237" s="16" t="str">
         <f ca="1">IF(Completed!A237&lt;&gt;"", IF(Completed!D237="", TODAY(), Completed!D237), "")</f>
         <v/>
       </c>
     </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D238" s="16" t="str">
         <f ca="1">IF(Completed!A238&lt;&gt;"", IF(Completed!D238="", TODAY(), Completed!D238), "")</f>
         <v/>
       </c>
     </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D239" s="16" t="str">
         <f ca="1">IF(Completed!A239&lt;&gt;"", IF(Completed!D239="", TODAY(), Completed!D239), "")</f>
         <v/>
       </c>
     </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D240" s="16" t="str">
         <f ca="1">IF(Completed!A240&lt;&gt;"", IF(Completed!D240="", TODAY(), Completed!D240), "")</f>
         <v/>
       </c>
     </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D241" s="16" t="str">
         <f ca="1">IF(Completed!A241&lt;&gt;"", IF(Completed!D241="", TODAY(), Completed!D241), "")</f>
         <v/>
       </c>
     </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D242" s="16" t="str">
         <f ca="1">IF(Completed!A242&lt;&gt;"", IF(Completed!D242="", TODAY(), Completed!D242), "")</f>
         <v/>
       </c>
     </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D243" s="16" t="str">
         <f ca="1">IF(Completed!A243&lt;&gt;"", IF(Completed!D243="", TODAY(), Completed!D243), "")</f>
         <v/>
       </c>
     </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D244" s="16" t="str">
         <f ca="1">IF(Completed!A244&lt;&gt;"", IF(Completed!D244="", TODAY(), Completed!D244), "")</f>
         <v/>
       </c>
     </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D245" s="16" t="str">
         <f ca="1">IF(Completed!A245&lt;&gt;"", IF(Completed!D245="", TODAY(), Completed!D245), "")</f>
         <v/>
       </c>
     </row>
-    <row r="246" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D246" s="16" t="str">
         <f ca="1">IF(Completed!A246&lt;&gt;"", IF(Completed!D246="", TODAY(), Completed!D246), "")</f>
         <v/>
       </c>
     </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D247" s="16" t="str">
         <f ca="1">IF(Completed!A247&lt;&gt;"", IF(Completed!D247="", TODAY(), Completed!D247), "")</f>
         <v/>
       </c>
     </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D248" s="16" t="str">
         <f ca="1">IF(Completed!A248&lt;&gt;"", IF(Completed!D248="", TODAY(), Completed!D248), "")</f>
         <v/>
       </c>
     </row>
-    <row r="249" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D249" s="16" t="str">
         <f ca="1">IF(Completed!A249&lt;&gt;"", IF(Completed!D249="", TODAY(), Completed!D249), "")</f>
         <v/>
       </c>
     </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D250" s="16" t="str">
         <f ca="1">IF(Completed!A250&lt;&gt;"", IF(Completed!D250="", TODAY(), Completed!D250), "")</f>
         <v/>
@@ -4818,24 +4842,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.1796875"/>
+    <col min="1" max="1025" width="8.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>